<commit_message>
Suma de Totales Final
</commit_message>
<xml_diff>
--- a/data/vmre.xlsx
+++ b/data/vmre.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,22 +15,11 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>estados</t>
   </si>
@@ -80,16 +69,43 @@
     <t>VOTOS_NULOS</t>
   </si>
   <si>
+    <t>Nayarit</t>
+  </si>
+  <si>
+    <t>MEC POSTAL</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>MEC INTERNET</t>
+  </si>
+  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Nayarit</t>
-  </si>
-  <si>
-    <t>MEC POSTAL</t>
-  </si>
-  <si>
-    <t>MEC INTERNET</t>
   </si>
 </sst>
 </file>
@@ -133,18 +149,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -169,7 +183,7 @@
     <tableColumn id="2" name="tipoMesa"/>
     <tableColumn id="3" name="numeroMesa"/>
     <tableColumn id="4" name="PAN"/>
-    <tableColumn id="5" name="PRI" dataDxfId="1"/>
+    <tableColumn id="5" name="PRI" dataDxfId="0"/>
     <tableColumn id="6" name="PRD"/>
     <tableColumn id="7" name="VERDE"/>
     <tableColumn id="8" name="PT"/>
@@ -181,9 +195,7 @@
     <tableColumn id="14" name="PT_MORENA"/>
     <tableColumn id="15" name="CANDIDATOS_NO_REGISTRADOS"/>
     <tableColumn id="16" name="VOTOS_NULOS"/>
-    <tableColumn id="17" name="Total" dataDxfId="0">
-      <calculatedColumnFormula>SUM(votosMRE[[#This Row],[VOTOS_NULOS]]+votosMRE[[#This Row],[CANDIDATOS_NO_REGISTRADOS]]+votosMRE[[#This Row],[PT_MORENA]]+votosMRE[[#This Row],[VERDE_MORENA]]+votosMRE[[#This Row],[VERDE_PT]]+votosMRE[[#This Row],[VERDE_PT_MORENA]]+votosMRE[[#This Row],[MORENA]]+votosMRE[[#This Row],[MOVIMIENTO_CIUDADANO]]+votosMRE[[#This Row],[PT]]+votosMRE[[#This Row],[VERDE]]+votosMRE[[#This Row],[PRD]]+votosMRE[[#This Row],[PRI]]+votosMRE[[#This Row],[PAN]])</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="19" name="Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -486,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,202 +571,124 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2">
-        <v>15</v>
-      </c>
-      <c r="N2" s="2">
-        <v>3</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1">
-        <f>SUM(C2:P2)</f>
-        <v>27</v>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <f t="shared" ref="D3:P3" si="0">SUBTOTAL(109,D2)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L3" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M3" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="N3" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="O3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <f>SUM(C3:P3)</f>
-        <v>27</v>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4">
-        <f>SUM(D2:D3)</f>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f>SUM(E2:E3)</f>
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <f>SUM(F2:F3)</f>
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <f>SUM(G2:G3)</f>
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <f>SUM(H2:H3)</f>
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <f>SUM(I2:I3)</f>
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <f>SUM(J2:J3)</f>
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <f>SUM(K2:K3)</f>
-        <v>8</v>
-      </c>
-      <c r="L4">
-        <f>SUM(L2:L3)</f>
-        <v>4</v>
-      </c>
-      <c r="M4">
-        <f>SUM(M2:M3)</f>
-        <v>30</v>
-      </c>
-      <c r="N4">
-        <f>SUM(N2:N3)</f>
-        <v>6</v>
-      </c>
-      <c r="O4">
-        <f>SUM(O2:O3)</f>
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <f>SUM(P2:P3)</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <f>SUM(Q2:Q3)</f>
-        <v>54</v>
-      </c>
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="2"/>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>